<commit_message>
neue rohdaten, plausibilitätsprüfung, cleaning
</commit_message>
<xml_diff>
--- a/raw/Plakate_1945-90_ImportCBS_Teil1.xlsx
+++ b/raw/Plakate_1945-90_ImportCBS_Teil1.xlsx
@@ -84,7 +84,7 @@
     <t xml:space="preserve">D</t>
   </si>
   <si>
-    <t xml:space="preserve">1 Blatt</t>
+    <t xml:space="preserve">1 ungezähltes Blatt</t>
   </si>
   <si>
     <t xml:space="preserve">Risse größer als 3 cm mit drohendem Materialverlust, Fehlstellen, stark brüchiges Papier</t>
@@ -213,7 +213,7 @@
     <t xml:space="preserve">1945-90/1007</t>
   </si>
   <si>
-    <t xml:space="preserve">Aufhängespuren, Einstempelung auf Vorderseite</t>
+    <t xml:space="preserve">Aufhängespuren,  Einstempelung auf Vorderseite</t>
   </si>
   <si>
     <t xml:space="preserve">1945-90/1008</t>
@@ -336,7 +336,7 @@
     <t xml:space="preserve">1945-90/1018</t>
   </si>
   <si>
-    <t xml:space="preserve">Beziehung zu 1945-90/1019, 1945-90/1032, 1945-90/1033 (Ausschneidebogen)</t>
+    <t xml:space="preserve">Beziehung zu 1945-90/1019, 1945-90/1032, 1945-90/1033  (Ausschneidebogen)</t>
   </si>
   <si>
     <t xml:space="preserve">P68/85b</t>
@@ -471,7 +471,7 @@
     <t xml:space="preserve">1945-90/1033</t>
   </si>
   <si>
-    <t xml:space="preserve">Beziehung zu 1945-90/1019, 1945-90/1032 (Ausschneidebogen)</t>
+    <t xml:space="preserve">Beziehung zu 1945-90/1019, 1945-90/1032  (Ausschneidebogen)</t>
   </si>
   <si>
     <t xml:space="preserve">P68/101</t>
@@ -2439,7 +2439,7 @@
     <t xml:space="preserve">1945-90/1264</t>
   </si>
   <si>
-    <t xml:space="preserve">Landkarte auf RS</t>
+    <t xml:space="preserve">Landkarte auf  RS</t>
   </si>
   <si>
     <t xml:space="preserve">P69/166</t>
@@ -2877,7 +2877,7 @@
     <t xml:space="preserve">14 Blätter</t>
   </si>
   <si>
-    <t xml:space="preserve">Mappenwerk; Faksimiles in Plastikfolie; 14 Objekte und 1 Umschlag mit Text</t>
+    <t xml:space="preserve">Mappenwerk; Faksimiles  in Plastikfolie; 14 Objekte und 1 Umschlag mit Text</t>
   </si>
   <si>
     <t xml:space="preserve">Ein Objekt im A-Format</t>
@@ -3003,7 +3003,7 @@
     <t xml:space="preserve">Serie mit Text und 33 Originalen; Beziehung zu 1322: große Ausgabe der Lenin-Serie</t>
   </si>
   <si>
-    <t xml:space="preserve">handschriftliche Notiz: Plakat 9 ausgeliehen nach Gotha: fehlt!</t>
+    <t xml:space="preserve">handschriftliche Notiz: Plakat 9  ausgeliehen nach Gotha: fehlt!</t>
   </si>
   <si>
     <t xml:space="preserve">1322,0-1 Riss &gt;3cm; 1322,34-1 Fehlstelle</t>
@@ -8466,7 +8466,7 @@
     <t xml:space="preserve">1945-90/786</t>
   </si>
   <si>
-    <t xml:space="preserve">handgeschrieben und handgezeichnet; diverse originale handschriftliche Unterschriften; Inhaltlicher Zusammenhang zwischen 785, 786 und 787 soll gewahrt werden </t>
+    <t xml:space="preserve">handgeschrieben und handgezeichnet; diverse originale handschriftliche Unterschriften;  Inhaltlicher Zusammenhang zwischen 785, 786 und 787 soll gewahrt werden </t>
   </si>
   <si>
     <t xml:space="preserve">P66/817</t>
@@ -8475,7 +8475,7 @@
     <t xml:space="preserve">1945-90/787</t>
   </si>
   <si>
-    <t xml:space="preserve">handgeschrieben und handgestaltete Wandzeitung; aufgeklebter Zeitungsartikel; diverse originale handschriftliche Unterschriften; Inhaltlicher Zusammenhang zwischen 785, 786 und 787 soll gewahrt werden </t>
+    <t xml:space="preserve">handgeschrieben und handgestaltete Wandzeitung; aufgeklebter Zeitungsartikel; diverse originale handschriftliche Unterschriften;  Inhaltlicher Zusammenhang zwischen 785, 786 und 787 soll gewahrt werden </t>
   </si>
   <si>
     <t xml:space="preserve">P66/818</t>
@@ -10127,7 +10127,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -10166,6 +10166,14 @@
       <charset val="1"/>
     </font>
     <font>
+      <b val="true"/>
+      <sz val="7"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="6"/>
       <name val="Verdana"/>
       <family val="2"/>
@@ -10187,7 +10195,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -10198,6 +10206,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFED7D31"/>
         <bgColor rgb="FFFF8080"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor rgb="FFFF0000"/>
       </patternFill>
     </fill>
     <fill>
@@ -10381,74 +10395,74 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -10456,11 +10470,11 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -10472,27 +10486,27 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="justify" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="justify" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="justify" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -10520,31 +10534,31 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -10552,15 +10566,15 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -10568,19 +10582,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -10588,71 +10602,71 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -10675,7 +10689,7 @@
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FFC00000"/>
       <rgbColor rgb="FF008000"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FF808000"/>
@@ -10735,10 +10749,10 @@
   </sheetPr>
   <dimension ref="A1:P1404"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="J11" activeCellId="0" sqref="J11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A164" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="P1" activeCellId="0" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.82421875" defaultRowHeight="7.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10758,7 +10772,7 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="16" style="9" width="12.82"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" s="14" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -10777,22 +10791,22 @@
       <c r="F1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="H1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="I1" s="11" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="14" t="s">
+      <c r="K1" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="14" t="s">
+      <c r="L1" s="13" t="s">
         <v>11</v>
       </c>
       <c r="M1" s="10" t="s">
@@ -23117,7 +23131,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="342" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="342" customFormat="false" ht="22.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A342" s="15" t="s">
         <v>15</v>
       </c>
@@ -23923,7 +23937,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="364" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="364" customFormat="false" ht="52.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A364" s="15" t="s">
         <v>15</v>
       </c>
@@ -26103,7 +26117,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="425" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="425" customFormat="false" ht="22.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A425" s="15" t="s">
         <v>15</v>
       </c>
@@ -26363,7 +26377,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="432" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="432" customFormat="false" ht="22.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A432" s="15" t="s">
         <v>15</v>
       </c>
@@ -27116,7 +27130,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="453" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="453" customFormat="false" ht="22.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A453" s="15" t="s">
         <v>15</v>
       </c>
@@ -27229,7 +27243,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="456" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="456" customFormat="false" ht="22.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A456" s="15" t="s">
         <v>15</v>
       </c>
@@ -27268,7 +27282,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="457" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="457" customFormat="false" ht="22.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A457" s="15" t="s">
         <v>15</v>
       </c>
@@ -27305,7 +27319,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="458" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="458" customFormat="false" ht="22.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A458" s="15" t="s">
         <v>15</v>
       </c>
@@ -27378,7 +27392,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="460" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="460" customFormat="false" ht="22.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A460" s="15" t="s">
         <v>15</v>
       </c>
@@ -37805,7 +37819,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="748" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="748" customFormat="false" ht="22.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A748" s="15" t="s">
         <v>15</v>
       </c>
@@ -40697,7 +40711,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="830" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="830" customFormat="false" ht="37.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A830" s="15" t="s">
         <v>15</v>
       </c>

</xml_diff>